<commit_message>
Added images and algorithmic design paradigms questions.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="260">
   <si>
     <t xml:space="preserve">Question Number</t>
   </si>
@@ -427,16 +427,450 @@
   </si>
   <si>
     <t xml:space="preserve">Knuth–Morris–Pratt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algorithmic Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using the Huffman Code, how many bits would you need to encode the word ‘Pneumonoultramicroscopicsilicovolcanokoniosis’?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201 bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">654 bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163 bits </t>
+  </si>
+  <si>
+    <t xml:space="preserve">871 bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppose you are trying to infiltrate as many computers as possible but you can only access one computer at a time. How fast you retrieve information from it depends on the computer’s start up processing time and finishing time. In sequence, which computers will you infiltrate to? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer 1 – Computer 3  – Computer 5 – Computer 2    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer 4 – Computer 6 – Computer 7 – Computer 2     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer 4  – Computer 1 – Computer 6 – computer 8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Computer 1 – Computer 4 - Computer  8  – Computer 6</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You come across a storage room filled with the latest high-tech gadgets and gizmos worth a lot of money. You’re tempted to take every single one but you only have one knapsack that could only fit 7 kilos of items so you take the items with the most value. How much more money could you have gained if you took a dynamic approach in selecting the items? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (this is the optimal solution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before you embarked on your journey, you bought the following items; gloves, knapsack, mask, a new pair of shoes, fake mustache, a beanie, &amp; some tools. The change given to you by the cashier was Php 230. Since it’s rush hour some of their coins and bills ran out, leaving only a set of pesos   {1, 10, 25, 50} to exchange with you. Using the greedy algorithm, what is the fewest number of peso bills/coins the cashier could have given you? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 50, 50, 50,50, 25,1,1,1,1,1}   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 50, 50, 50,50, 10,10,10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 50, 50, 50,25, 1,1,1,1,1,25,25}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{50, 50, 25, 25, 25, 25, 10, 10, 10}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are assigned to be the leader of the hacking operation. To execute the task effectively you split your members into pairs. However, most of your members agrees to be paired with a partner according to their preference. What one stable match could you think of? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{(M1,M6), (M2,M5), (M3,M8), (M4,M7)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{(M1,M6), (M2,M7), (M3,M5), (M4,M8)} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{(M1,M8), (M2,M5), (M3,M6), (M4,M7)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{(M1,M7), (M2,M8), (M3,M5), (M4,M6)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When does a greedy algorithm produce an optimal solution to a problem? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a global optimal solution can be found by choosing the optimal solution at each step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When it finds a global optimal solution by recursively trying to build a solution incrementally, one piece at a time, recursively evaluating every alternative and choosing the best one. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If it evaluates each and every possibility until it finds the global optimal solution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If an optimal solution can be created for a problem by constructing optimal solutions for its sub problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You tried to access one of the main computers of the surveillance room but the computer only registers the password when spoken. Knowing the password by using a password-cracking software you whisper the words, “A miss is as good as a mile” but the computer completely misheard you with “I kiss as good as my wife”. To remedy this error find the minimum edit distance of these two strings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the length of the Longest Common Subsequence for the strings “29381049284” and “18249018383”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the length of the Longest Increasing Subsequence for the set {23,10,3,19,-1,2,0,1,39,18,38,11,13,18,27,32,-6,8,7}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many subsets within the set {9,4,8,1,7,5,3} has a sum of 12? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why is Dynamic Programming a much preferred approach in solving optimization problems compared to greedy algorithms? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because Greedy algorithms never work!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because Dynamic Programming has a faster time complexity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because it is more efficient in memory space. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because it considers all possible cases and then chooses the best. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is true? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic programming is recursion with repetition. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A greedy algorithm constructs a solution with a series of decisions with solving at any recursive subproblems. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The algorithm for the Fibonacci sequence with Dynamic Programming is O(2^n). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems involving an optimal substructure and overlapping subproblems can be best solved by Dynamic Programming </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Find the errors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF242021"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in the execution steps of the linear search algorithm implemented</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Line 3, 11, 27, 29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line 5, 10, 11, 29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line 3, 5, 10, 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line 5, 11, 27, 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using insertion sort, which among the following are the steps of insertions done to the array, arr[5] = {12,10,8,6,4,2}?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 10 8 6 2 4 12 10 8 2 4 6 12 10 2 4 6 8 12 2 4 6 8 10 2 4 6 8 10 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 8 6 4 2 12 8 6 4 2 10 12 6 4 2 8 10 12 4 2 6 8 10 12 2 4 6 8 10 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 12 8 6 4 2 4 12 8 6 2 4 6 12 8 2 4 6 8 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 12 8 6 4 2 6 8 10 12 4 2 2 6 8 10 12 4 2 4 6 8 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using insertion sort to sort the array, arr[5]= {5,8,2,1,6,7,12,-1}, what is the total cost of the insertion sort when element -1 reaches the first position of the array if at each insertion the cost would be 2 pesos?   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following describes the Linear Search algorithm? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time taken to search elements keep decreasing as the number of elements are increased.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It scans one item at a time, without jumping at any item </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It has a time complexity of O(n^2) for integer data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It does not access data sequentially. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When is Linear Search preferred over other searching algorithms? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When dealing with sorted data sets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In cases where there is a large data set. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When data keeps changing frequently </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both a and b.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What advantages can you get by using Brute Force algorithms? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The brute force approach guarantees that it will always find a correct solution to a problem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The brute force method is ideal for solving large and simpler problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brute force approach is fast and efficient. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of the above. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_______ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">finds solution(s) by trying all possible paths and then abandoning them if they are not suitable.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Greedy Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic Programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhaustive Search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backtracking Paradigm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a chess board having 4 x 4 cells, we need to place 4 queens in such a way that no queen is attacked by any other queen. A queen can attack horizontally, vertically and diagonally. How many times will you backtrack to get all the possible solutions? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is NOT part of the strategy of the backtracking paradigm? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extending a partial solution in some feasible way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trying another extension if the extension fails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backing up to a smaller partial solution when the options for extending a partial solution are exhausted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">randomly explore the space of all potential solutions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Considering the list of integers {4,6,2} , which of the following demonstrates the backtracking approach of finding a subset with sum 6? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ } -&gt; {4} -&gt; {4, 6} (found) -&gt; {4} -&gt;{4,2} (found) -&gt; {4} (end) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ } -&gt; {4} -&gt; {4, 6} (found) -&gt; {4,6,2} (found) -&gt; (end) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{4} -&gt; {4, 6} (found) -&gt; {4} -&gt; {4,2} (found) -&gt; { } (end)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ } -&gt; {4} -&gt; {4, 6} (found) -&gt; {4} -&gt; {4, 2} (found) -&gt; {4,6}, {4,2} (end)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which among these choices is NOT a valid step for the Divide and Conquer paradigm? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine the solutions of the sub-problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Break down the problem into smaller sub-problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store the sub-problem solutions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solve the separate sub-problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppose you encounter the  Tower of Hanoi puzzle wherein there are 3 rods where an entire stack of 4 disks must move to another rod (in this case rod C) following these rules:  1) Only one disk can be moved at a time. 2) Each move consists of taking the upper disk from one of the stacks and placing it on top of another stack i.e. a disk can only be moved if it is the uppermost disk on a stack. 3.) No disk may be placed on top of a smaller disk. Using the minimum number of moves to solve this step, what is a possible move for the 13th step? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move biggest disk from rod A to rod B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move third disk from rod A to rod B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move second disk from rod A to rod B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move smallest disk from rod A to rod B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppose vertex 1 is the school’s library and the other vertices are the school’s departments. The library is locked but you remembered you saw the librarian handing the keys to an assistant professor but you don’t know which department. You think of the possible minimum path to visit all of the school’s departments however lunch break is almost over so you took the naïve approach of finding the minimum path. According to your approach how many possible paths are there to go from the library to the school’s departments and back to the library again along with distance of the minimum path? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 paths &amp; minimum distance of 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 paths &amp; minimum distance of 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 paths &amp; minimum distance of 19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 paths &amp; minimum distance of 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determine the correct order of the following sorting algorithms according to their time efficiency. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insertion Sort  &lt; Merge Sort  &lt; Quick Sort </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Sort  &lt; Quick Sort &lt;  Selection Sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selection Sort &lt;  Heap Sort &lt; Insertion Sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Sort  &lt; Merge Sort &lt; Heap Sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the most important “building blocks” you should understand to help you in designing algorithms?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algorithmic Techniques, Data Structures and Proof techniques </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structures, Time complexity and Space Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrix Multiplication, Fast Fourier Transform and O-notation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic Programming, Recursion and Brute force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The keys Mike, May, Ren, Nat, Rey, Carl, Nico, Bri, Joan, and Steph are inserted into an initially empty hash table of length 10 using open addressing with hash function h(k) = k mod 10 and linear probing. What key(s) is/are in index 7 in the hash table?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyze the given program below and indicate it’s time complexity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O(n^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two robots are competing against each other on a sorting match. They have to sort these 10 items {football, baseball, golf ball, volleyball, bowling ball, soccer ball, tennis ball, billiard ball, ping pong,  basketball } from heaviest to lightest. Robot 1 will sort the items using merge sort and Robot 2, quick sort. Who will win the match and how many comparisons did the loser do? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winner is Merge Sort and loser does 21 comparisons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winner is Quick Sort and loser does 22 comparisons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winner is Merge Sort and loser does 23 comparisons. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winner is Quick Sort and loser does 24 comparisons </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -460,10 +894,52 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242021"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF273239"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -508,7 +984,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,12 +993,64 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -534,7 +1062,183 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF242021"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF273239"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>563760</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>101880</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Picture 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5127480" y="13741560"/>
+          <a:ext cx="153360" cy="176760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>454320</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>137880</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6248520" y="13741560"/>
+          <a:ext cx="298800" cy="176760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>442080</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31320</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6851520" y="13741560"/>
+          <a:ext cx="204480" cy="207360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,13 +1246,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.24"/>
   </cols>
@@ -1587,7 +2291,7 @@
       <c r="B36" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -1616,7 +2320,7 @@
       <c r="B37" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D37" s="0" t="s">
@@ -1801,7 +2505,7 @@
       <c r="B44" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D44" s="0" t="s">
@@ -1859,10 +2563,10 @@
       <c r="B46" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E46" s="0" t="s">
@@ -1879,6 +2583,867 @@
       </c>
       <c r="J46" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E49" s="7" t="n">
+        <v>26000</v>
+      </c>
+      <c r="F49" s="7" t="n">
+        <v>16000</v>
+      </c>
+      <c r="G49" s="7" t="n">
+        <v>36000</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E53" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="F53" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E54" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F54" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G54" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="G55" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D56" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F56" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G56" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F61" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G61" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E66" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="F66" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G66" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H69" s="4"/>
+      <c r="J69" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1889,5 +3454,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added intractability questions, added resources for algo design and intractability.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="397">
   <si>
     <t xml:space="preserve">Question Number</t>
   </si>
@@ -484,6 +484,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">/Images/AlgoD_Item2_Image.PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">MEDIUM</t>
   </si>
   <si>
@@ -493,6 +496,9 @@
     <t xml:space="preserve">0 (this is the optimal solution)</t>
   </si>
   <si>
+    <t xml:space="preserve">/Images/AlgoD_Item3_Image.PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Before you embarked on your journey, you bought the following items; gloves, knapsack, mask, a new pair of shoes, fake mustache, a beanie, &amp; some tools. The change given to you by the cashier was Php 230. Since it’s rush hour some of their coins and bills ran out, leaving only a set of pesos   {1, 10, 25, 50} to exchange with you. Using the greedy algorithm, what is the fewest number of peso bills/coins the cashier could have given you? </t>
   </si>
   <si>
@@ -521,6 +527,9 @@
   </si>
   <si>
     <t xml:space="preserve">{(M1,M7), (M2,M8), (M3,M5), (M4,M6)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/AlgoD_Item5_Image.PNG</t>
   </si>
   <si>
     <t xml:space="preserve">When does a greedy algorithm produce an optimal solution to a problem? </t>
@@ -612,6 +621,9 @@
   </si>
   <si>
     <t xml:space="preserve">Line 5, 11, 27, 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/AlgoD_Item13_Image.PNG</t>
   </si>
   <si>
     <t xml:space="preserve">Using insertion sort, which among the following are the steps of insertions done to the array, arr[5] = {12,10,8,6,4,2}?</t>
@@ -778,6 +790,9 @@
     <t xml:space="preserve">Move smallest disk from rod A to rod B </t>
   </si>
   <si>
+    <t xml:space="preserve">/Images/AlgoD_Item24_Image.PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suppose vertex 1 is the school’s library and the other vertices are the school’s departments. The library is locked but you remembered you saw the librarian handing the keys to an assistant professor but you don’t know which department. You think of the possible minimum path to visit all of the school’s departments however lunch break is almost over so you took the naïve approach of finding the minimum path. According to your approach how many possible paths are there to go from the library to the school’s departments and back to the library again along with distance of the minimum path? </t>
   </si>
   <si>
@@ -793,6 +808,9 @@
     <t xml:space="preserve">7 paths &amp; minimum distance of 25</t>
   </si>
   <si>
+    <t xml:space="preserve">/Images/AlgoD_Item25_Image.PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Determine the correct order of the following sorting algorithms according to their time efficiency. </t>
   </si>
   <si>
@@ -847,6 +865,9 @@
     <t xml:space="preserve"> O(n^2)</t>
   </si>
   <si>
+    <t xml:space="preserve">/Images/AlgoD_Item29_Image.PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two robots are competing against each other on a sorting match. They have to sort these 10 items {football, baseball, golf ball, volleyball, bowling ball, soccer ball, tennis ball, billiard ball, ping pong,  basketball } from heaviest to lightest. Robot 1 will sort the items using merge sort and Robot 2, quick sort. Who will win the match and how many comparisons did the loser do? </t>
   </si>
   <si>
@@ -860,6 +881,470 @@
   </si>
   <si>
     <t xml:space="preserve">Winner is Quick Sort and loser does 24 comparisons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/AlgoD_Item30_Image.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intractability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> How many possible solutions are there for a 9 Queen’s Puzzle? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following positions for a queen on a 4 X 4 board is part of a solution of a 4 Queen’s Puzzle? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A queen positioned at row 2, column 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A queen positioned at row 3, column 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A queen positioned at row 1, column 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A queen positioned at row 4, column 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIUM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppose we’re given an Adjacency Matrix of Graph G (where 0 indicates that the vertex[column] is not connected to the vertex [row] and 1 indicates it is connected to the vertex) and we need to color its 6 vertices using only a maximum of 3 colors where no two adjacent vertices share the same color. What’s one way to color this graph in sequence? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color 1, Color 1, Color 2, Color 1, Color 3, Color 3, Color 1, Color 2, Color 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color 1, Color 2, Color 1, Color 2, Color 1, Color 3, Color 1, Color 3, Color 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color 1, Color 2, Color 3, Color 1, Color 2, Color 1, Color 1, Color 3, Color 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color 1, Color 1, Color 2, Color 3, Color 2, Color 1, Color 1, Color 2, Color 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item3pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the many applications for the graph coloring problem is solving a Sudoku puzzle where the vertices represents the squares of the grid and each number within the squares are connected by an edge to another number that lies within the same row, column or 2x2 grid and must be colored differently from each other. Suppose we have a 2 x 2 box that has characters 1 to 4, how many edges does this graph have? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item4pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a table for pairs of subjects that one or more students are taking together (colored in green), suppose that you are tasked to schedule exams so that there will be no possible conflicts between students taking the subjects.  What timeslots will be possible for scheduling student exams?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeslot B, C &amp; E    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeslot A &amp; D  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeslot C &amp; E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timeslot A, C &amp; D    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item5pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the maximum clique given a graph with V vertices and E edges V = 8, Edges[][] = {{A,B},{A,C},{B,C},{B,F},{B,D},{C,D},{C,F},{D,E},{D,H},{E,F},{E,G},{E,H},{F,G},{G,H}}? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On accessing a website, a CAPTCHA suddenly pops up and asks you to color this abstract image as few colors as possible in such a way that no shape of the same color shares the same border. It seems as though CAPTCHA’s way of verifying if you’re a human or not is getting a bit complicated but still, how many colors will you use? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item7pic.PNG</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Using the greedy algorithm given, what is the correct order of coloring the vertices that would provide the fewest possible colors in coloring graph G with </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> vertices and </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> edges </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">V </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">= 10, Edges[][] = {{0,1},{0,5},(0,6},{1,2},{1,7},{2,3},{2,5},{3,4},{3,8},{4,5},{4,9},{5,6},{5,9}{6,7},{6,9},{7,8},{8,9}?</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of vertices: V0, V1, V2, V3, V4, V5, V9, V8, V7, V6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of vertices: V0, V6, V9, V4, V5, V2, V3, V8, V7, V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of vertices: V0, V5, V4, V3, V2, V1, V7, V8, V9, V6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of vertices: V0, V1, V7, V6, V5, V2, V3, V8, V9, V4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item8pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are given a layout of the building you’re trying to break in.  Suppose that it also has the possible locations where the school would put the CCTV cameras so that they have surveillances in each area using only a minimum number of cameras. On the map, the cameras are indicated in vertices and the edges represent the direction(s) the camera can face. Find out how many CCTV cameras you need to look out for.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 8 CCTV Cameras installed in the building. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 5 CCTV Cameras installed in the building.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 6 CCTV Cameras installed in the building. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 9 CCTV Cameras installed in the building.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item9pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We’re given an algorithm for solving the vertex cover of a graph. Suppose our graph G with V vertices &amp; E edges V = 8, Edges[][], {{A,B},{A,J},{A,F},{B,J},{B,C},{C,I},{C,D},{D,I},{D,E},{E,F},{E,G},{F,G},{G,H},{H,I},{H,J}} 
+is given. Which of the following is not a solution? 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = [B,J,I,D,F,G]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = [A,B,I,C,E,D,G,H]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = [A,B,I,C,E,D,F,G,H,J]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = [A,B,E,D,F,G,H,J]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item10pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give a truth assignment that satisfies the given Boolean expression. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item11pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transcribe this Boolean circuit as a Boolean formula. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item12pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is the satisfiable 3CNF formula that represents the graph of this maximum independent set? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item13pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What satisfiable 3CNF formula is the given 3-colorable graph derived from?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item14pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a graph of a maximum independent set, how many vertices will you need to find the minimum vertex cover? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item15pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why does the question of whether P = NP matters?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It matters because of the million dollar reward and fame you’ll attain when you correctly prove it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It hasn’t been proven or disproven for nearly 5 decades now, it matters because of man’s quest for solving the unknown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If P = NP then we can easily solve seemingly hard problems. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If P = NP then we can determine which kinds of problems are solvable by computers and which ones are not. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which theorem proved that Circuit satisfiability is NP-hard? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramsey Theorem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cook-Levin Theorem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Four Color Theorem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brook’s Theorem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Sudoku puzzle has been shown to be ______? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP-hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is not an intractable problem? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tower of Hanoi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching an unordered list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling Salesman Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A _____ is a problem whose output is a single Boolean value. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turing reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision problem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph coloring problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subset sum problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following has been proven?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP ≠ EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P ≠ EXP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP ≠ co-NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P = NP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following order of these complexity classes is correct?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P⊆NP⊆PSPACE⊆EXP⊆NEXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P⊆NP⊆EXP⊆NEXP⊆PSPACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP⊆P⊆NEXP⊆EXP⊆PSPACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P⊆NP⊆PSPACE⊆NEXP⊆EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is NOT part of  the general pattern in polynomial-time reductions?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform an arbitrary for y into a certificate of y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prove that if x is a “good” instance of X, then y is a “good” instance of Y. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prove that if y is a “good” instance of Y, then x is a “good” instance of X.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe a polynomial-time algorithm to transform an arbitrary instance x of X into a special instance y of Y.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is false? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems in P are easy to solve and easy to verify its solution. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems in NP may or may not be hard to solve but easy to verify its solution. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An algorithm is considered efficient if &amp; only if it can run at polynomial time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there is proof that one NP-complete problem is impossible to solve, then we cannot solve P vs NP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How will you classify if a problem is NP hard? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If it is impossible to find an efficient algorithm to solve the problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the problem is hard to solve but its solution can be easily verified.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the problem is both NP-complete and NP-easy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you can easily reduce a known NP-hard problem to the current problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When is a problem considered NP-complete?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there is a polynomial-time algorithm for every problem in NP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a problem is both NP-hard and NP-easy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If every decision problem in P is also in NP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the solution to the problem can be verified in polynomial-time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the problem asks to find a small subset satisfying some constraints, what best suitable NP-complete problem will you reduce this from? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CircuitSat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinVertexCover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxClique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What will NOT happen if you found a polynomial-time algorithm for an NP-complete problem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will gain fame and fortune.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All your private information on the internet will be easily accessed.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will impose severe limits on what computers can accomplish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’ll wake up to find that it is possible to cure cancer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following information describes why this given diagram is incorrect? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P⊆NP,P⊆coNP,NP≠coNP,NPcomplete ⊆NP &amp; NPhard ⊆NP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P ≠coNP,P⊆NP,coNP⊆NP,NPcomplete ⊆NP &amp; NPhard ⊆coNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coNP⊆NP,P≠NP,NP⊆NPhard &amp; NPhard ⊆Npcomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P⊆NP,P⊆coNP,NP≠coNP,NPcomplete ⊆NP &amp; NPcomplete ⊆Nphard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/Intractability_item29pic.PNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of these problems do not have a polynomial-time algorithm?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N x N Queen’s puzzle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All NP-complete problems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling salesman problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of the above. </t>
   </si>
 </sst>
 </file>
@@ -902,12 +1387,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -939,6 +1418,14 @@
       <color rgb="FF273239"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -984,7 +1471,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1009,15 +1496,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1025,27 +1508,27 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1130,15 +1613,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>563760</xdr:colOff>
+      <xdr:colOff>565920</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>101880</xdr:colOff>
+      <xdr:colOff>103320</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1151,8 +1634,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5127480" y="13741560"/>
-          <a:ext cx="153360" cy="176760"/>
+          <a:off x="5130720" y="13678560"/>
+          <a:ext cx="153360" cy="174600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1167,15 +1650,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>454320</xdr:colOff>
+      <xdr:colOff>455760</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>137880</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1188,8 +1671,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6248520" y="13741560"/>
-          <a:ext cx="298800" cy="176760"/>
+          <a:off x="6252480" y="13678560"/>
+          <a:ext cx="298800" cy="174600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1204,15 +1687,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>442080</xdr:colOff>
+      <xdr:colOff>443160</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>31320</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:colOff>32040</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1225,8 +1708,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6851520" y="13741560"/>
-          <a:ext cx="204480" cy="207360"/>
+          <a:off x="6855840" y="13678560"/>
+          <a:ext cx="204840" cy="205200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1246,13 +1729,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L101" activeCellId="0" sqref="L101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.24"/>
   </cols>
@@ -2586,6 +3069,9 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
       <c r="B47" s="1" t="s">
         <v>135</v>
       </c>
@@ -2636,8 +3122,11 @@
       <c r="H48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="I48" s="4" t="s">
         <v>147</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,25 +3137,28 @@
         <v>135</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="E49" s="6" t="n">
         <v>26000</v>
       </c>
-      <c r="F49" s="7" t="n">
+      <c r="F49" s="6" t="n">
         <v>16000</v>
       </c>
-      <c r="G49" s="7" t="n">
+      <c r="G49" s="6" t="n">
         <v>36000</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I49" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="J49" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,19 +3169,19 @@
         <v>135</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>22</v>
@@ -2706,25 +3198,28 @@
         <v>135</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="I51" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="J51" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,19 +3230,19 @@
         <v>135</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>22</v>
@@ -2764,7 +3259,7 @@
         <v>135</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D53" s="4" t="n">
         <v>7</v>
@@ -2782,7 +3277,7 @@
         <v>16</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,7 +3288,7 @@
         <v>135</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>8</v>
@@ -2811,7 +3306,7 @@
         <v>27</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,8 +3316,8 @@
       <c r="B55" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>167</v>
+      <c r="C55" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>8</v>
@@ -2851,7 +3346,7 @@
         <v>135</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>3</v>
@@ -2880,19 +3375,19 @@
         <v>135</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>27</v>
@@ -2909,19 +3404,19 @@
         <v>135</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>27</v>
@@ -2937,23 +3432,26 @@
       <c r="B59" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>179</v>
+      <c r="C59" s="10" t="s">
+        <v>182</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>17</v>
@@ -2967,19 +3465,19 @@
         <v>135</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>51</v>
@@ -2996,7 +3494,7 @@
         <v>135</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D61" s="4" t="n">
         <v>2</v>
@@ -3014,7 +3512,7 @@
         <v>27</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,25 +3523,25 @@
         <v>135</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3054,25 +3552,25 @@
         <v>135</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3082,26 +3580,26 @@
       <c r="B64" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="11" t="s">
-        <v>201</v>
+      <c r="C64" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,26 +3609,26 @@
       <c r="B65" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>206</v>
+      <c r="C65" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>27</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,7 +3639,7 @@
         <v>135</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D66" s="4" t="n">
         <v>10</v>
@@ -3170,19 +3668,19 @@
         <v>135</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>27</v>
@@ -3199,25 +3697,25 @@
         <v>135</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,19 +3726,19 @@
         <v>135</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="H69" s="4"/>
       <c r="J69" s="1" t="s">
@@ -3255,24 +3753,27 @@
         <v>135</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="F70" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="G70" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="H70" s="13" t="s">
+      <c r="D70" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="H70" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J70" s="14" t="s">
+      <c r="I70" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="J70" s="13" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3284,25 +3785,28 @@
         <v>135</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="I71" s="4" t="s">
+        <v>242</v>
+      </c>
       <c r="J71" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3313,19 +3817,19 @@
         <v>135</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>22</v>
@@ -3341,25 +3845,25 @@
       <c r="B73" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C73" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H73" s="10" t="s">
+      <c r="C73" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H73" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J73" s="11" t="s">
+      <c r="J73" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3371,25 +3875,25 @@
         <v>135</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>51</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3399,19 +3903,22 @@
       <c r="B75" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="16" t="s">
-        <v>252</v>
+      <c r="C75" s="15" t="s">
+        <v>258</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>51</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="J75" s="0" t="s">
         <v>17</v>
@@ -3425,25 +3932,893 @@
         <v>135</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="I76" s="4" t="s">
+        <v>267</v>
+      </c>
       <c r="J76" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D77" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="E77" s="4" t="n">
+        <v>92</v>
+      </c>
+      <c r="F77" s="4" t="n">
+        <v>352</v>
+      </c>
+      <c r="G77" s="4" t="n">
+        <v>545</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D91" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E91" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F91" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G91" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added metaheuristic algo questions 1-12 with resources.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="495">
   <si>
     <t xml:space="preserve">Question Number</t>
   </si>
@@ -1576,6 +1576,69 @@
   </si>
   <si>
     <t xml:space="preserve">/Images/SA3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metaheuristic Algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following image contains code that is part of the implementation of the Firefly Algorithm written in Python. Which part in the general procedure of swarm intelligence algorithms is the shown code?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population Initialization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluate all initialized individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reproduce individuals to form a new population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluate the fitness of each solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update solutions in the archive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select solutions with better fitness values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following image contains code that is part of the implementation of the Firefly Algorithm written in Java. Which part in the general procedure of swarm intelligence algorithms is the shown code?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA10.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA11.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Images/MA12.png</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1785,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="12" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1730,7 +1793,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="12" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1854,15 +1917,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>565920</xdr:colOff>
+      <xdr:colOff>566280</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>103320</xdr:colOff>
+      <xdr:colOff>102960</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1875,8 +1938,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5132160" y="13678920"/>
-          <a:ext cx="153720" cy="173880"/>
+          <a:off x="5133600" y="13679280"/>
+          <a:ext cx="154080" cy="173160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1891,15 +1954,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>456120</xdr:colOff>
+      <xdr:colOff>456480</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>138240</xdr:colOff>
+      <xdr:colOff>137880</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1912,8 +1975,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6255360" y="13678920"/>
-          <a:ext cx="298800" cy="173880"/>
+          <a:off x="6258240" y="13679280"/>
+          <a:ext cx="298800" cy="173160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1930,13 +1993,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>443160</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>31680</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1949,8 +2012,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6859080" y="13678920"/>
-          <a:ext cx="205200" cy="204480"/>
+          <a:off x="6862320" y="13679280"/>
+          <a:ext cx="205560" cy="203760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1970,13 +2033,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I120" activeCellId="0" sqref="I120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C134" activeCellId="0" sqref="C134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.24"/>
   </cols>
@@ -5063,6 +5126,9 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
       <c r="B107" s="0" t="s">
         <v>104</v>
       </c>
@@ -5089,7 +5155,10 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="16" t="s">
+      <c r="A108" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C108" s="0" t="s">
@@ -5115,7 +5184,10 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="16" t="s">
+      <c r="A109" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C109" s="0" t="s">
@@ -5141,7 +5213,10 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="16" t="s">
+      <c r="A110" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C110" s="0" t="s">
@@ -5167,7 +5242,10 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="16" t="s">
+      <c r="A111" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C111" s="0" t="s">
@@ -5193,7 +5271,10 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="16" t="s">
+      <c r="A112" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C112" s="0" t="s">
@@ -5219,7 +5300,10 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="16" t="s">
+      <c r="A113" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C113" s="0" t="s">
@@ -5245,7 +5329,10 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="16" t="s">
+      <c r="A114" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C114" s="0" t="s">
@@ -5271,7 +5358,10 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="16" t="s">
+      <c r="A115" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C115" s="0" t="s">
@@ -5297,7 +5387,10 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="16" t="s">
+      <c r="A116" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C116" s="0" t="s">
@@ -5323,7 +5416,10 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="16" t="s">
+      <c r="A117" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C117" s="0" t="s">
@@ -5349,7 +5445,10 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="16" t="s">
+      <c r="A118" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C118" s="0" t="s">
@@ -5375,7 +5474,10 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="16" t="s">
+      <c r="A119" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C119" s="0" t="s">
@@ -5396,7 +5498,7 @@
       <c r="H119" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I119" s="16" t="s">
+      <c r="I119" s="1" t="s">
         <v>461</v>
       </c>
       <c r="J119" s="0" t="s">
@@ -5404,7 +5506,10 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="16" t="s">
+      <c r="A120" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C120" s="0" t="s">
@@ -5425,7 +5530,7 @@
       <c r="H120" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I120" s="16" t="s">
+      <c r="I120" s="1" t="s">
         <v>467</v>
       </c>
       <c r="J120" s="0" t="s">
@@ -5433,7 +5538,10 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="16" t="s">
+      <c r="A121" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C121" s="0" t="s">
@@ -5454,13 +5562,399 @@
       <c r="H121" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I121" s="16" t="s">
+      <c r="I121" s="1" t="s">
         <v>473</v>
       </c>
       <c r="J121" s="0" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="H122" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I122" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H123" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I123" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="J123" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H124" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I124" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="J124" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H125" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I125" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="J125" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="H126" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J126" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="H127" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I127" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="J127" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="H128" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I128" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="J128" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H129" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I129" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="J129" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H130" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="J130" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H131" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I131" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="J131" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="H132" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="J132" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="H133" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="J133" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>